<commit_message>
Updated and integrated new data
</commit_message>
<xml_diff>
--- a/files/Calvert_phyto.xlsx
+++ b/files/Calvert_phyto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20376"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justin.belluz\Documents\R\microscopy_OBIS\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DE9DCB-F1FA-4EB4-B744-BAD42505454B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6DD59F-54AF-439B-BA05-3E43C963C49E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13380" activeTab="6" xr2:uid="{097FCDEB-8C97-4367-A565-6CEADFA41F06}"/>
   </bookViews>
@@ -23,7 +23,7 @@
     <sheet name="DFO2_3" sheetId="8" r:id="rId8"/>
     <sheet name="DFO2_4" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1861" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="298">
   <si>
     <t>Bacillariophyta</t>
   </si>
@@ -987,6 +987,15 @@
   <si>
     <t>CPHY539</t>
   </si>
+  <si>
+    <t>CPHY534</t>
+  </si>
+  <si>
+    <t>CPHY537</t>
+  </si>
+  <si>
+    <t>CPHY540</t>
+  </si>
 </sst>
 </file>
 
@@ -19451,15 +19460,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670708D3-8086-459A-8CCF-F66DE9B4A94E}">
-  <dimension ref="A1:L221"/>
+  <dimension ref="A1:N221"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>230</v>
       </c>
@@ -19481,16 +19490,28 @@
       <c r="J1" s="12" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K1" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>200</v>
       </c>
@@ -19505,9 +19526,12 @@
         <v>40</v>
       </c>
       <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
       <c r="L3" s="12"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
@@ -19520,9 +19544,12 @@
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
       <c r="L4" s="12"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
@@ -19535,9 +19562,12 @@
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
       <c r="L5" s="12"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
@@ -19552,9 +19582,12 @@
       <c r="J6" s="12">
         <v>3500</v>
       </c>
+      <c r="K6" s="12"/>
       <c r="L6" s="12"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
@@ -19567,9 +19600,12 @@
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
       <c r="L7" s="12"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>6</v>
       </c>
@@ -19582,9 +19618,12 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
       <c r="L8" s="12"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
@@ -19599,9 +19638,14 @@
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
+      <c r="K9" s="12">
+        <v>1110</v>
+      </c>
       <c r="L9" s="12"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>201</v>
       </c>
@@ -19614,9 +19658,12 @@
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
       <c r="L10" s="12"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
@@ -19633,9 +19680,14 @@
       <c r="J11" s="12">
         <v>666</v>
       </c>
+      <c r="K11" s="12">
+        <v>111</v>
+      </c>
       <c r="L11" s="12"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>9</v>
       </c>
@@ -19654,9 +19706,12 @@
       <c r="J12" s="12">
         <v>7881</v>
       </c>
+      <c r="K12" s="12"/>
       <c r="L12" s="12"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>10</v>
       </c>
@@ -19671,9 +19726,12 @@
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
       <c r="L13" s="12"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>11</v>
       </c>
@@ -19686,9 +19744,12 @@
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
       <c r="L14" s="12"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>12</v>
       </c>
@@ -19701,9 +19762,12 @@
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
       <c r="L15" s="12"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>13</v>
       </c>
@@ -19716,9 +19780,12 @@
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
       <c r="L16" s="12"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>14</v>
       </c>
@@ -19735,9 +19802,12 @@
       </c>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
       <c r="L17" s="12"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>15</v>
       </c>
@@ -19758,9 +19828,14 @@
       <c r="J18" s="12">
         <v>60334</v>
       </c>
+      <c r="K18" s="12">
+        <v>20200</v>
+      </c>
       <c r="L18" s="12"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>16</v>
       </c>
@@ -19773,9 +19848,12 @@
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
       <c r="L19" s="12"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>17</v>
       </c>
@@ -19792,9 +19870,12 @@
       <c r="J20" s="12">
         <v>1110</v>
       </c>
+      <c r="K20" s="12"/>
       <c r="L20" s="12"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>18</v>
       </c>
@@ -19809,9 +19890,12 @@
       <c r="J21" s="12">
         <v>3108</v>
       </c>
+      <c r="K21" s="12"/>
       <c r="L21" s="12"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>19</v>
       </c>
@@ -19824,9 +19908,12 @@
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
       <c r="L22" s="12"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>20</v>
       </c>
@@ -19841,9 +19928,12 @@
       <c r="J23" s="12">
         <v>666</v>
       </c>
+      <c r="K23" s="12"/>
       <c r="L23" s="12"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>21</v>
       </c>
@@ -19860,9 +19950,14 @@
       <c r="J24" s="12">
         <v>777</v>
       </c>
+      <c r="K24" s="12">
+        <v>444</v>
+      </c>
       <c r="L24" s="12"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
         <v>22</v>
       </c>
@@ -19875,9 +19970,12 @@
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
       <c r="L25" s="12"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
         <v>23</v>
       </c>
@@ -19890,9 +19988,12 @@
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
       <c r="L26" s="12"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
         <v>24</v>
       </c>
@@ -19909,9 +20010,12 @@
       <c r="J27" s="12">
         <v>1554</v>
       </c>
+      <c r="K27" s="12"/>
       <c r="L27" s="12"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>25</v>
       </c>
@@ -19928,9 +20032,14 @@
       <c r="J28" s="12">
         <v>2664</v>
       </c>
+      <c r="K28" s="12">
+        <v>2220</v>
+      </c>
       <c r="L28" s="12"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
         <v>26</v>
       </c>
@@ -19943,9 +20052,12 @@
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
       <c r="L29" s="12"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
         <v>27</v>
       </c>
@@ -19960,9 +20072,14 @@
       <c r="J30" s="12">
         <v>666</v>
       </c>
+      <c r="K30" s="12">
+        <v>1110</v>
+      </c>
       <c r="L30" s="12"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
         <v>28</v>
       </c>
@@ -19975,9 +20092,12 @@
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
       <c r="L31" s="12"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
         <v>29</v>
       </c>
@@ -19996,9 +20116,12 @@
       <c r="J32" s="12">
         <v>2331</v>
       </c>
+      <c r="K32" s="12"/>
       <c r="L32" s="12"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="12" t="s">
         <v>30</v>
       </c>
@@ -20017,9 +20140,16 @@
       <c r="J33" s="12">
         <v>1332</v>
       </c>
-      <c r="L33" s="12"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K33" s="12">
+        <v>555</v>
+      </c>
+      <c r="L33" s="12">
+        <v>40</v>
+      </c>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
         <v>31</v>
       </c>
@@ -20032,9 +20162,12 @@
       <c r="H34" s="12"/>
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
       <c r="L34" s="12"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
         <v>32</v>
       </c>
@@ -20049,9 +20182,12 @@
       <c r="H35" s="12"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
       <c r="L35" s="12"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
         <v>33</v>
       </c>
@@ -20072,9 +20208,12 @@
       <c r="J36" s="12">
         <v>555</v>
       </c>
+      <c r="K36" s="12"/>
       <c r="L36" s="12"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>34</v>
       </c>
@@ -20093,9 +20232,14 @@
       <c r="J37" s="12">
         <v>111</v>
       </c>
-      <c r="L37" s="12"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K37" s="12"/>
+      <c r="L37" s="12">
+        <v>40</v>
+      </c>
+      <c r="M37" s="12"/>
+      <c r="N37" s="12"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>35</v>
       </c>
@@ -20118,9 +20262,14 @@
       <c r="J38" s="12">
         <v>14000</v>
       </c>
-      <c r="L38" s="12"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K38" s="12"/>
+      <c r="L38" s="12">
+        <v>3182</v>
+      </c>
+      <c r="M38" s="12"/>
+      <c r="N38" s="12"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
         <v>36</v>
       </c>
@@ -20135,9 +20284,12 @@
         <v>40</v>
       </c>
       <c r="J39" s="12"/>
+      <c r="K39" s="12"/>
       <c r="L39" s="12"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M39" s="12"/>
+      <c r="N39" s="12"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
         <v>37</v>
       </c>
@@ -20150,9 +20302,12 @@
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
+      <c r="K40" s="12"/>
       <c r="L40" s="12"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M40" s="12"/>
+      <c r="N40" s="12"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>38</v>
       </c>
@@ -20167,9 +20322,12 @@
       <c r="J41" s="12">
         <v>111</v>
       </c>
+      <c r="K41" s="12"/>
       <c r="L41" s="12"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
         <v>39</v>
       </c>
@@ -20194,9 +20352,18 @@
       <c r="J42" s="12">
         <v>2220</v>
       </c>
-      <c r="L42" s="12"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K42" s="12">
+        <v>222</v>
+      </c>
+      <c r="L42" s="12">
+        <v>40</v>
+      </c>
+      <c r="M42" s="12">
+        <v>40</v>
+      </c>
+      <c r="N42" s="12"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
         <v>40</v>
       </c>
@@ -20217,9 +20384,16 @@
       <c r="J43" s="12">
         <v>333</v>
       </c>
+      <c r="K43" s="12">
+        <v>444</v>
+      </c>
       <c r="L43" s="12"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M43" s="12">
+        <v>80</v>
+      </c>
+      <c r="N43" s="12"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
         <v>41</v>
       </c>
@@ -20236,9 +20410,12 @@
       <c r="H44" s="12"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
+      <c r="K44" s="12"/>
       <c r="L44" s="12"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M44" s="12"/>
+      <c r="N44" s="12"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="12" t="s">
         <v>42</v>
       </c>
@@ -20257,9 +20434,12 @@
       <c r="J45" s="12">
         <v>111</v>
       </c>
+      <c r="K45" s="12"/>
       <c r="L45" s="12"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M45" s="12"/>
+      <c r="N45" s="12"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="12" t="s">
         <v>43</v>
       </c>
@@ -20274,9 +20454,16 @@
       <c r="H46" s="12"/>
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
-      <c r="L46" s="12"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K46" s="12">
+        <v>2331</v>
+      </c>
+      <c r="L46" s="12">
+        <v>160</v>
+      </c>
+      <c r="M46" s="12"/>
+      <c r="N46" s="12"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
         <v>202</v>
       </c>
@@ -20289,9 +20476,12 @@
       <c r="H47" s="12"/>
       <c r="I47" s="12"/>
       <c r="J47" s="12"/>
+      <c r="K47" s="12"/>
       <c r="L47" s="12"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M47" s="12"/>
+      <c r="N47" s="12"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
         <v>44</v>
       </c>
@@ -20304,9 +20494,14 @@
       <c r="H48" s="12"/>
       <c r="I48" s="12"/>
       <c r="J48" s="12"/>
+      <c r="K48" s="12">
+        <v>555</v>
+      </c>
       <c r="L48" s="12"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M48" s="12"/>
+      <c r="N48" s="12"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="12" t="s">
         <v>45</v>
       </c>
@@ -20319,9 +20514,16 @@
       <c r="H49" s="12"/>
       <c r="I49" s="12"/>
       <c r="J49" s="12"/>
+      <c r="K49" s="12">
+        <v>2220</v>
+      </c>
       <c r="L49" s="12"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M49" s="12">
+        <v>40</v>
+      </c>
+      <c r="N49" s="12"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
         <v>46</v>
       </c>
@@ -20334,9 +20536,12 @@
       <c r="H50" s="12"/>
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
+      <c r="K50" s="12"/>
       <c r="L50" s="12"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M50" s="12"/>
+      <c r="N50" s="12"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="12" t="s">
         <v>47</v>
       </c>
@@ -20349,9 +20554,12 @@
       <c r="H51" s="12"/>
       <c r="I51" s="12"/>
       <c r="J51" s="12"/>
+      <c r="K51" s="12"/>
       <c r="L51" s="12"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M51" s="12"/>
+      <c r="N51" s="12"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
         <v>48</v>
       </c>
@@ -20368,9 +20576,12 @@
       <c r="H52" s="12"/>
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
+      <c r="K52" s="12"/>
       <c r="L52" s="12"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M52" s="12"/>
+      <c r="N52" s="12"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="12" t="s">
         <v>203</v>
       </c>
@@ -20383,9 +20594,12 @@
       <c r="H53" s="12"/>
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
+      <c r="K53" s="12"/>
       <c r="L53" s="12"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M53" s="12"/>
+      <c r="N53" s="12"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
         <v>49</v>
       </c>
@@ -20398,9 +20612,12 @@
       <c r="H54" s="12"/>
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
+      <c r="K54" s="12"/>
       <c r="L54" s="12"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M54" s="12"/>
+      <c r="N54" s="12"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="12" t="s">
         <v>50</v>
       </c>
@@ -20415,9 +20632,12 @@
       <c r="H55" s="12"/>
       <c r="I55" s="12"/>
       <c r="J55" s="12"/>
+      <c r="K55" s="12"/>
       <c r="L55" s="12"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M55" s="12"/>
+      <c r="N55" s="12"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="12" t="s">
         <v>51</v>
       </c>
@@ -20430,9 +20650,12 @@
       <c r="H56" s="12"/>
       <c r="I56" s="12"/>
       <c r="J56" s="12"/>
+      <c r="K56" s="12"/>
       <c r="L56" s="12"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M56" s="12"/>
+      <c r="N56" s="12"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="12" t="s">
         <v>52</v>
       </c>
@@ -20445,9 +20668,12 @@
       <c r="H57" s="12"/>
       <c r="I57" s="12"/>
       <c r="J57" s="12"/>
+      <c r="K57" s="12"/>
       <c r="L57" s="12"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M57" s="12"/>
+      <c r="N57" s="12"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="12" t="s">
         <v>53</v>
       </c>
@@ -20460,9 +20686,12 @@
       <c r="H58" s="12"/>
       <c r="I58" s="12"/>
       <c r="J58" s="12"/>
+      <c r="K58" s="12"/>
       <c r="L58" s="12"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M58" s="12"/>
+      <c r="N58" s="12"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="12" t="s">
         <v>54</v>
       </c>
@@ -20475,9 +20704,12 @@
       <c r="H59" s="12"/>
       <c r="I59" s="12"/>
       <c r="J59" s="12"/>
+      <c r="K59" s="12"/>
       <c r="L59" s="12"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M59" s="12"/>
+      <c r="N59" s="12"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="12" t="s">
         <v>55</v>
       </c>
@@ -20490,9 +20722,12 @@
       <c r="H60" s="12"/>
       <c r="I60" s="12"/>
       <c r="J60" s="12"/>
+      <c r="K60" s="12"/>
       <c r="L60" s="12"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M60" s="12"/>
+      <c r="N60" s="12"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="12" t="s">
         <v>56</v>
       </c>
@@ -20507,9 +20742,12 @@
       <c r="H61" s="12"/>
       <c r="I61" s="12"/>
       <c r="J61" s="12"/>
+      <c r="K61" s="12"/>
       <c r="L61" s="12"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M61" s="12"/>
+      <c r="N61" s="12"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="12" t="s">
         <v>57</v>
       </c>
@@ -20526,9 +20764,12 @@
       <c r="J62" s="12">
         <v>111</v>
       </c>
+      <c r="K62" s="12"/>
       <c r="L62" s="12"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M62" s="12"/>
+      <c r="N62" s="12"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="12" t="s">
         <v>58</v>
       </c>
@@ -20549,9 +20790,12 @@
         <v>640</v>
       </c>
       <c r="J63" s="12"/>
+      <c r="K63" s="12"/>
       <c r="L63" s="12"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M63" s="12"/>
+      <c r="N63" s="12"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" s="12" t="s">
         <v>59</v>
       </c>
@@ -20572,9 +20816,18 @@
       <c r="J64" s="12">
         <v>666</v>
       </c>
-      <c r="L64" s="12"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K64" s="12">
+        <v>222</v>
+      </c>
+      <c r="L64" s="12">
+        <v>160</v>
+      </c>
+      <c r="M64" s="12">
+        <v>160</v>
+      </c>
+      <c r="N64" s="12"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" s="12" t="s">
         <v>60</v>
       </c>
@@ -20591,9 +20844,14 @@
       <c r="H65" s="12"/>
       <c r="I65" s="12"/>
       <c r="J65" s="12"/>
+      <c r="K65" s="12">
+        <v>222</v>
+      </c>
       <c r="L65" s="12"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M65" s="12"/>
+      <c r="N65" s="12"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" s="12" t="s">
         <v>61</v>
       </c>
@@ -20608,9 +20866,14 @@
         <v>40</v>
       </c>
       <c r="J66" s="12"/>
+      <c r="K66" s="12">
+        <v>222</v>
+      </c>
       <c r="L66" s="12"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M66" s="12"/>
+      <c r="N66" s="12"/>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" s="12" t="s">
         <v>61</v>
       </c>
@@ -20625,9 +20888,12 @@
       <c r="H67" s="12"/>
       <c r="I67" s="12"/>
       <c r="J67" s="12"/>
+      <c r="K67" s="12"/>
       <c r="L67" s="12"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M67" s="12"/>
+      <c r="N67" s="12"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" s="12" t="s">
         <v>62</v>
       </c>
@@ -20650,9 +20916,16 @@
       <c r="J68" s="12">
         <v>121360</v>
       </c>
-      <c r="L68" s="12"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K68" s="12">
+        <v>268000</v>
+      </c>
+      <c r="L68" s="12">
+        <v>2200</v>
+      </c>
+      <c r="M68" s="12"/>
+      <c r="N68" s="12"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" s="12" t="s">
         <v>63</v>
       </c>
@@ -20677,9 +20950,18 @@
       <c r="J69" s="12">
         <v>162000</v>
       </c>
-      <c r="L69" s="12"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K69" s="12">
+        <v>118400</v>
+      </c>
+      <c r="L69" s="12">
+        <v>5002</v>
+      </c>
+      <c r="M69" s="12">
+        <v>280</v>
+      </c>
+      <c r="N69" s="12"/>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" s="12" t="s">
         <v>204</v>
       </c>
@@ -20694,9 +20976,12 @@
         <v>80</v>
       </c>
       <c r="J70" s="12"/>
+      <c r="K70" s="12"/>
       <c r="L70" s="12"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M70" s="12"/>
+      <c r="N70" s="12"/>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" s="12" t="s">
         <v>64</v>
       </c>
@@ -20709,9 +20994,12 @@
       <c r="H71" s="12"/>
       <c r="I71" s="12"/>
       <c r="J71" s="12"/>
+      <c r="K71" s="12"/>
       <c r="L71" s="12"/>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M71" s="12"/>
+      <c r="N71" s="12"/>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" s="12" t="s">
         <v>65</v>
       </c>
@@ -20726,9 +21014,12 @@
       <c r="H72" s="12"/>
       <c r="I72" s="12"/>
       <c r="J72" s="12"/>
+      <c r="K72" s="12"/>
       <c r="L72" s="12"/>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M72" s="12"/>
+      <c r="N72" s="12"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" s="12" t="s">
         <v>66</v>
       </c>
@@ -20753,9 +21044,16 @@
       <c r="J73" s="12">
         <v>1332</v>
       </c>
-      <c r="L73" s="12"/>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K73" s="12">
+        <v>4662</v>
+      </c>
+      <c r="L73" s="12">
+        <v>80</v>
+      </c>
+      <c r="M73" s="12"/>
+      <c r="N73" s="12"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" s="12" t="s">
         <v>67</v>
       </c>
@@ -20768,9 +21066,12 @@
       <c r="H74" s="12"/>
       <c r="I74" s="12"/>
       <c r="J74" s="12"/>
+      <c r="K74" s="12"/>
       <c r="L74" s="12"/>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M74" s="12"/>
+      <c r="N74" s="12"/>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" s="12" t="s">
         <v>68</v>
       </c>
@@ -20789,9 +21090,14 @@
       <c r="J75" s="12">
         <v>37000</v>
       </c>
+      <c r="K75" s="12">
+        <v>3330</v>
+      </c>
       <c r="L75" s="12"/>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M75" s="12"/>
+      <c r="N75" s="12"/>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" s="12" t="s">
         <v>69</v>
       </c>
@@ -20808,9 +21114,12 @@
       <c r="J76" s="12">
         <v>59200</v>
       </c>
+      <c r="K76" s="12"/>
       <c r="L76" s="12"/>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M76" s="12"/>
+      <c r="N76" s="12"/>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" s="12" t="s">
         <v>70</v>
       </c>
@@ -20827,9 +21136,14 @@
       <c r="J77" s="12">
         <v>666</v>
       </c>
+      <c r="K77" s="12">
+        <v>1776</v>
+      </c>
       <c r="L77" s="12"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M77" s="12"/>
+      <c r="N77" s="12"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" s="12" t="s">
         <v>71</v>
       </c>
@@ -20854,9 +21168,18 @@
       <c r="J78" s="12">
         <v>28600</v>
       </c>
-      <c r="L78" s="12"/>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K78" s="12">
+        <v>2997</v>
+      </c>
+      <c r="L78" s="12">
+        <v>200</v>
+      </c>
+      <c r="M78" s="12">
+        <v>80</v>
+      </c>
+      <c r="N78" s="12"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" s="12" t="s">
         <v>72</v>
       </c>
@@ -20871,9 +21194,12 @@
       <c r="H79" s="12"/>
       <c r="I79" s="12"/>
       <c r="J79" s="12"/>
+      <c r="K79" s="12"/>
       <c r="L79" s="12"/>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M79" s="12"/>
+      <c r="N79" s="12"/>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" s="12" t="s">
         <v>73</v>
       </c>
@@ -20888,9 +21214,16 @@
       </c>
       <c r="I80" s="12"/>
       <c r="J80" s="12"/>
-      <c r="L80" s="12"/>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K80" s="12">
+        <v>777</v>
+      </c>
+      <c r="L80" s="12">
+        <v>80</v>
+      </c>
+      <c r="M80" s="12"/>
+      <c r="N80" s="12"/>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" s="12" t="s">
         <v>74</v>
       </c>
@@ -20913,9 +21246,14 @@
       <c r="J81" s="12">
         <v>52500</v>
       </c>
+      <c r="K81" s="12"/>
       <c r="L81" s="12"/>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M81" s="12">
+        <v>1750</v>
+      </c>
+      <c r="N81" s="12"/>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" s="12" t="s">
         <v>75</v>
       </c>
@@ -20940,9 +21278,18 @@
       <c r="J82" s="12">
         <v>1443</v>
       </c>
-      <c r="L82" s="12"/>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K82" s="12">
+        <v>333</v>
+      </c>
+      <c r="L82" s="12">
+        <v>80</v>
+      </c>
+      <c r="M82" s="12">
+        <v>200</v>
+      </c>
+      <c r="N82" s="12"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" s="12" t="s">
         <v>76</v>
       </c>
@@ -20961,9 +21308,16 @@
       </c>
       <c r="I83" s="12"/>
       <c r="J83" s="12"/>
-      <c r="L83" s="12"/>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K83" s="12">
+        <v>5000</v>
+      </c>
+      <c r="L83" s="12">
+        <v>3182</v>
+      </c>
+      <c r="M83" s="12"/>
+      <c r="N83" s="12"/>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" s="12" t="s">
         <v>77</v>
       </c>
@@ -20976,9 +21330,12 @@
       <c r="H84" s="12"/>
       <c r="I84" s="12"/>
       <c r="J84" s="12"/>
+      <c r="K84" s="12"/>
       <c r="L84" s="12"/>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M84" s="12"/>
+      <c r="N84" s="12"/>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85" s="12" t="s">
         <v>78</v>
       </c>
@@ -21009,9 +21366,21 @@
         <f t="shared" si="0"/>
         <v>568908</v>
       </c>
-      <c r="L85" s="12"/>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K85" s="12">
+        <f t="shared" ref="K85:M85" si="1">SUM(K3:K84)</f>
+        <v>437463</v>
+      </c>
+      <c r="L85" s="12">
+        <f t="shared" si="1"/>
+        <v>14446</v>
+      </c>
+      <c r="M85" s="12">
+        <f t="shared" si="1"/>
+        <v>2630</v>
+      </c>
+      <c r="N85" s="12"/>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86" s="12"/>
       <c r="B86" s="12"/>
       <c r="C86" s="12"/>
@@ -21022,9 +21391,12 @@
       <c r="H86" s="12"/>
       <c r="I86" s="12"/>
       <c r="J86" s="12"/>
+      <c r="K86" s="12"/>
       <c r="L86" s="12"/>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M86" s="12"/>
+      <c r="N86" s="12"/>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87" s="13" t="s">
         <v>79</v>
       </c>
@@ -21037,9 +21409,12 @@
       <c r="H87" s="12"/>
       <c r="I87" s="12"/>
       <c r="J87" s="12"/>
+      <c r="K87" s="12"/>
       <c r="L87" s="12"/>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M87" s="12"/>
+      <c r="N87" s="12"/>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88" s="12" t="s">
         <v>80</v>
       </c>
@@ -21052,9 +21427,12 @@
       <c r="H88" s="12"/>
       <c r="I88" s="12"/>
       <c r="J88" s="12"/>
+      <c r="K88" s="12"/>
       <c r="L88" s="12"/>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M88" s="12"/>
+      <c r="N88" s="12"/>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89" s="12" t="s">
         <v>81</v>
       </c>
@@ -21075,9 +21453,14 @@
       </c>
       <c r="I89" s="12"/>
       <c r="J89" s="12"/>
+      <c r="K89" s="12">
+        <v>5000</v>
+      </c>
       <c r="L89" s="12"/>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M89" s="12"/>
+      <c r="N89" s="12"/>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" s="12" t="s">
         <v>82</v>
       </c>
@@ -21092,9 +21475,12 @@
       <c r="H90" s="12"/>
       <c r="I90" s="12"/>
       <c r="J90" s="12"/>
+      <c r="K90" s="12"/>
       <c r="L90" s="12"/>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M90" s="12"/>
+      <c r="N90" s="12"/>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91" s="12" t="s">
         <v>83</v>
       </c>
@@ -21111,9 +21497,16 @@
         <v>2917</v>
       </c>
       <c r="J91" s="12"/>
-      <c r="L91" s="12"/>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K91" s="12">
+        <v>5000</v>
+      </c>
+      <c r="L91" s="12">
+        <v>3182</v>
+      </c>
+      <c r="M91" s="12"/>
+      <c r="N91" s="12"/>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92" s="12" t="s">
         <v>84</v>
       </c>
@@ -21138,9 +21531,16 @@
       <c r="J92" s="12">
         <v>14000</v>
       </c>
-      <c r="L92" s="12"/>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K92" s="12">
+        <v>25000</v>
+      </c>
+      <c r="L92" s="12">
+        <v>12728</v>
+      </c>
+      <c r="M92" s="12"/>
+      <c r="N92" s="12"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93" s="12" t="s">
         <v>85</v>
       </c>
@@ -21153,9 +21553,12 @@
       <c r="H93" s="12"/>
       <c r="I93" s="12"/>
       <c r="J93" s="12"/>
+      <c r="K93" s="12"/>
       <c r="L93" s="12"/>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M93" s="12"/>
+      <c r="N93" s="12"/>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94" s="12" t="s">
         <v>86</v>
       </c>
@@ -21168,9 +21571,12 @@
       <c r="H94" s="12"/>
       <c r="I94" s="12"/>
       <c r="J94" s="12"/>
+      <c r="K94" s="12"/>
       <c r="L94" s="12"/>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M94" s="12"/>
+      <c r="N94" s="12"/>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95" s="12" t="s">
         <v>87</v>
       </c>
@@ -21195,9 +21601,18 @@
       <c r="J95" s="12">
         <v>42000</v>
       </c>
-      <c r="L95" s="12"/>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K95" s="12">
+        <v>185000</v>
+      </c>
+      <c r="L95" s="12">
+        <v>85914</v>
+      </c>
+      <c r="M95" s="12">
+        <v>14000</v>
+      </c>
+      <c r="N95" s="12"/>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96" s="12"/>
       <c r="B96" s="12"/>
       <c r="C96" s="12"/>
@@ -21208,9 +21623,12 @@
       <c r="H96" s="12"/>
       <c r="I96" s="12"/>
       <c r="J96" s="12"/>
+      <c r="K96" s="12"/>
       <c r="L96" s="12"/>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M96" s="12"/>
+      <c r="N96" s="12"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A97" s="13" t="s">
         <v>88</v>
       </c>
@@ -21223,9 +21641,12 @@
       <c r="H97" s="12"/>
       <c r="I97" s="12"/>
       <c r="J97" s="12"/>
+      <c r="K97" s="12"/>
       <c r="L97" s="12"/>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M97" s="12"/>
+      <c r="N97" s="12"/>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98" s="12" t="s">
         <v>89</v>
       </c>
@@ -21238,9 +21659,12 @@
       <c r="H98" s="12"/>
       <c r="I98" s="12"/>
       <c r="J98" s="12"/>
+      <c r="K98" s="12"/>
       <c r="L98" s="12"/>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M98" s="12"/>
+      <c r="N98" s="12"/>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A99" s="12" t="s">
         <v>90</v>
       </c>
@@ -21255,9 +21679,12 @@
       <c r="J99" s="12">
         <v>10500</v>
       </c>
+      <c r="K99" s="12"/>
       <c r="L99" s="12"/>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M99" s="12"/>
+      <c r="N99" s="12"/>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A100" s="12" t="s">
         <v>91</v>
       </c>
@@ -21276,9 +21703,14 @@
       <c r="J100" s="12">
         <v>14000</v>
       </c>
+      <c r="K100" s="12">
+        <v>5000</v>
+      </c>
       <c r="L100" s="12"/>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M100" s="12"/>
+      <c r="N100" s="12"/>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A101" s="12" t="s">
         <v>92</v>
       </c>
@@ -21293,9 +21725,12 @@
       <c r="H101" s="12"/>
       <c r="I101" s="12"/>
       <c r="J101" s="12"/>
+      <c r="K101" s="12"/>
       <c r="L101" s="12"/>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M101" s="12"/>
+      <c r="N101" s="12"/>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A102" s="12" t="s">
         <v>87</v>
       </c>
@@ -21320,9 +21755,18 @@
       <c r="J102" s="12">
         <v>70000</v>
       </c>
-      <c r="L102" s="12"/>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K102" s="12">
+        <v>65000</v>
+      </c>
+      <c r="L102" s="12">
+        <v>38184</v>
+      </c>
+      <c r="M102" s="12">
+        <v>3500</v>
+      </c>
+      <c r="N102" s="12"/>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A103" s="12"/>
       <c r="B103" s="12"/>
       <c r="C103" s="12"/>
@@ -21333,9 +21777,12 @@
       <c r="H103" s="12"/>
       <c r="I103" s="12"/>
       <c r="J103" s="12"/>
+      <c r="K103" s="12"/>
       <c r="L103" s="12"/>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M103" s="12"/>
+      <c r="N103" s="12"/>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A104" s="13" t="s">
         <v>93</v>
       </c>
@@ -21348,9 +21795,12 @@
       <c r="H104" s="12"/>
       <c r="I104" s="12"/>
       <c r="J104" s="12"/>
+      <c r="K104" s="12"/>
       <c r="L104" s="12"/>
-    </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M104" s="12"/>
+      <c r="N104" s="12"/>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A105" s="12" t="s">
         <v>94</v>
       </c>
@@ -21365,9 +21815,12 @@
       <c r="J105" s="12">
         <v>3500</v>
       </c>
+      <c r="K105" s="12"/>
       <c r="L105" s="12"/>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M105" s="12"/>
+      <c r="N105" s="12"/>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A106" s="12" t="s">
         <v>205</v>
       </c>
@@ -21380,9 +21833,12 @@
       <c r="H106" s="12"/>
       <c r="I106" s="12"/>
       <c r="J106" s="12"/>
+      <c r="K106" s="12"/>
       <c r="L106" s="12"/>
-    </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M106" s="12"/>
+      <c r="N106" s="12"/>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A107" s="12" t="s">
         <v>206</v>
       </c>
@@ -21397,9 +21853,12 @@
         <v>2917</v>
       </c>
       <c r="J107" s="12"/>
+      <c r="K107" s="12"/>
       <c r="L107" s="12"/>
-    </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M107" s="12"/>
+      <c r="N107" s="12"/>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A108" s="12" t="s">
         <v>87</v>
       </c>
@@ -21412,9 +21871,12 @@
       <c r="H108" s="12"/>
       <c r="I108" s="12"/>
       <c r="J108" s="12"/>
+      <c r="K108" s="12"/>
       <c r="L108" s="12"/>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M108" s="12"/>
+      <c r="N108" s="12"/>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A109" s="12"/>
       <c r="B109" s="12"/>
       <c r="C109" s="12"/>
@@ -21425,9 +21887,12 @@
       <c r="H109" s="12"/>
       <c r="I109" s="12"/>
       <c r="J109" s="12"/>
+      <c r="K109" s="12"/>
       <c r="L109" s="12"/>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M109" s="12"/>
+      <c r="N109" s="12"/>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A110" s="13" t="s">
         <v>97</v>
       </c>
@@ -21440,9 +21905,12 @@
       <c r="H110" s="12"/>
       <c r="I110" s="12"/>
       <c r="J110" s="12"/>
+      <c r="K110" s="12"/>
       <c r="L110" s="12"/>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M110" s="12"/>
+      <c r="N110" s="12"/>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A111" s="12" t="s">
         <v>98</v>
       </c>
@@ -21457,9 +21925,12 @@
         <v>40</v>
       </c>
       <c r="J111" s="12"/>
+      <c r="K111" s="12"/>
       <c r="L111" s="12"/>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M111" s="12"/>
+      <c r="N111" s="12"/>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A112" s="12" t="s">
         <v>99</v>
       </c>
@@ -21484,9 +21955,18 @@
       <c r="J112" s="12">
         <v>333</v>
       </c>
-      <c r="L112" s="12"/>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K112" s="12">
+        <v>1443</v>
+      </c>
+      <c r="L112" s="12">
+        <v>560</v>
+      </c>
+      <c r="M112" s="12">
+        <v>320</v>
+      </c>
+      <c r="N112" s="12"/>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A113" s="12" t="s">
         <v>100</v>
       </c>
@@ -21511,9 +21991,18 @@
       <c r="J113" s="12">
         <v>888</v>
       </c>
-      <c r="L113" s="12"/>
-    </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K113" s="12">
+        <v>1776</v>
+      </c>
+      <c r="L113" s="12">
+        <v>800</v>
+      </c>
+      <c r="M113" s="12">
+        <v>200</v>
+      </c>
+      <c r="N113" s="12"/>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A114" s="12" t="s">
         <v>101</v>
       </c>
@@ -21526,9 +22015,12 @@
       <c r="H114" s="12"/>
       <c r="I114" s="12"/>
       <c r="J114" s="12"/>
+      <c r="K114" s="12"/>
       <c r="L114" s="12"/>
-    </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M114" s="12"/>
+      <c r="N114" s="12"/>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A115" s="12" t="s">
         <v>102</v>
       </c>
@@ -21553,9 +22045,18 @@
       <c r="J115" s="12">
         <v>1887</v>
       </c>
-      <c r="L115" s="12"/>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K115" s="12">
+        <v>2997</v>
+      </c>
+      <c r="L115" s="12">
+        <v>1960</v>
+      </c>
+      <c r="M115" s="12">
+        <v>520</v>
+      </c>
+      <c r="N115" s="12"/>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A116" s="12" t="s">
         <v>103</v>
       </c>
@@ -21572,9 +22073,16 @@
         <v>40</v>
       </c>
       <c r="J116" s="12"/>
-      <c r="L116" s="12"/>
-    </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K116" s="12">
+        <v>555</v>
+      </c>
+      <c r="L116" s="12">
+        <v>80</v>
+      </c>
+      <c r="M116" s="12"/>
+      <c r="N116" s="12"/>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A117" s="12"/>
       <c r="B117" s="12"/>
       <c r="C117" s="12"/>
@@ -21585,9 +22093,12 @@
       <c r="H117" s="12"/>
       <c r="I117" s="12"/>
       <c r="J117" s="12"/>
+      <c r="K117" s="12"/>
       <c r="L117" s="12"/>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M117" s="12"/>
+      <c r="N117" s="12"/>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A118" s="13" t="s">
         <v>104</v>
       </c>
@@ -21600,9 +22111,12 @@
       <c r="H118" s="12"/>
       <c r="I118" s="12"/>
       <c r="J118" s="12"/>
+      <c r="K118" s="12"/>
       <c r="L118" s="12"/>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M118" s="12"/>
+      <c r="N118" s="12"/>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A119" s="12" t="s">
         <v>105</v>
       </c>
@@ -21627,9 +22141,18 @@
       <c r="J119" s="12">
         <v>91000</v>
       </c>
-      <c r="L119" s="12"/>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K119" s="12">
+        <v>215000</v>
+      </c>
+      <c r="L119" s="12">
+        <v>95460</v>
+      </c>
+      <c r="M119" s="12">
+        <v>10500</v>
+      </c>
+      <c r="N119" s="12"/>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A120" s="12" t="s">
         <v>106</v>
       </c>
@@ -21644,9 +22167,14 @@
       <c r="H120" s="12"/>
       <c r="I120" s="12"/>
       <c r="J120" s="12"/>
-      <c r="L120" s="12"/>
-    </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K120" s="12"/>
+      <c r="L120" s="12">
+        <v>3182</v>
+      </c>
+      <c r="M120" s="12"/>
+      <c r="N120" s="12"/>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A121" s="12" t="s">
         <v>107</v>
       </c>
@@ -21659,9 +22187,16 @@
       <c r="H121" s="12"/>
       <c r="I121" s="12"/>
       <c r="J121" s="12"/>
-      <c r="L121" s="12"/>
-    </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K121" s="12">
+        <v>10000</v>
+      </c>
+      <c r="L121" s="12">
+        <v>3182</v>
+      </c>
+      <c r="M121" s="12"/>
+      <c r="N121" s="12"/>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A122" s="12" t="s">
         <v>108</v>
       </c>
@@ -21686,9 +22221,18 @@
       <c r="J122" s="12">
         <v>52500</v>
       </c>
-      <c r="L122" s="12"/>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K122" s="12">
+        <v>190000</v>
+      </c>
+      <c r="L122" s="12">
+        <v>66822</v>
+      </c>
+      <c r="M122" s="12">
+        <v>8750</v>
+      </c>
+      <c r="N122" s="12"/>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A123" s="12"/>
       <c r="B123" s="12"/>
       <c r="C123" s="12"/>
@@ -21699,9 +22243,12 @@
       <c r="H123" s="12"/>
       <c r="I123" s="12"/>
       <c r="J123" s="12"/>
+      <c r="K123" s="12"/>
       <c r="L123" s="12"/>
-    </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M123" s="12"/>
+      <c r="N123" s="12"/>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A124" s="12" t="s">
         <v>109</v>
       </c>
@@ -21714,9 +22261,12 @@
       <c r="H124" s="12"/>
       <c r="I124" s="12"/>
       <c r="J124" s="12"/>
+      <c r="K124" s="12"/>
       <c r="L124" s="12"/>
-    </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M124" s="12"/>
+      <c r="N124" s="12"/>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A125" s="12"/>
       <c r="B125" s="12"/>
       <c r="C125" s="12"/>
@@ -21727,9 +22277,12 @@
       <c r="H125" s="12"/>
       <c r="I125" s="12"/>
       <c r="J125" s="12"/>
+      <c r="K125" s="12"/>
       <c r="L125" s="12"/>
-    </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M125" s="12"/>
+      <c r="N125" s="12"/>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A126" s="13" t="s">
         <v>110</v>
       </c>
@@ -21742,9 +22295,12 @@
       <c r="H126" s="12"/>
       <c r="I126" s="12"/>
       <c r="J126" s="12"/>
+      <c r="K126" s="12"/>
       <c r="L126" s="12"/>
-    </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M126" s="12"/>
+      <c r="N126" s="12"/>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A127" s="12" t="s">
         <v>111</v>
       </c>
@@ -21761,9 +22317,14 @@
       <c r="J127" s="12">
         <v>111</v>
       </c>
+      <c r="K127" s="12">
+        <v>111</v>
+      </c>
       <c r="L127" s="12"/>
-    </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M127" s="12"/>
+      <c r="N127" s="12"/>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A128" s="12" t="s">
         <v>112</v>
       </c>
@@ -21776,9 +22337,14 @@
       <c r="H128" s="12"/>
       <c r="I128" s="12"/>
       <c r="J128" s="12"/>
+      <c r="K128" s="12">
+        <v>111</v>
+      </c>
       <c r="L128" s="12"/>
-    </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M128" s="12"/>
+      <c r="N128" s="12"/>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A129" s="12" t="s">
         <v>113</v>
       </c>
@@ -21791,9 +22357,12 @@
       <c r="H129" s="12"/>
       <c r="I129" s="12"/>
       <c r="J129" s="12"/>
+      <c r="K129" s="12"/>
       <c r="L129" s="12"/>
-    </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M129" s="12"/>
+      <c r="N129" s="12"/>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A130" s="12" t="s">
         <v>114</v>
       </c>
@@ -21816,9 +22385,18 @@
         <v>360</v>
       </c>
       <c r="J130" s="12"/>
-      <c r="L130" s="12"/>
-    </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K130" s="12">
+        <v>333</v>
+      </c>
+      <c r="L130" s="12">
+        <v>160</v>
+      </c>
+      <c r="M130" s="12">
+        <v>40</v>
+      </c>
+      <c r="N130" s="12"/>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A131" s="12" t="s">
         <v>115</v>
       </c>
@@ -21833,9 +22411,16 @@
       </c>
       <c r="I131" s="12"/>
       <c r="J131" s="12"/>
-      <c r="L131" s="12"/>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K131" s="12">
+        <v>2775</v>
+      </c>
+      <c r="L131" s="12">
+        <v>440</v>
+      </c>
+      <c r="M131" s="12"/>
+      <c r="N131" s="12"/>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A132" s="12" t="s">
         <v>116</v>
       </c>
@@ -21852,9 +22437,12 @@
       <c r="J132" s="12">
         <v>3500</v>
       </c>
+      <c r="K132" s="12"/>
       <c r="L132" s="12"/>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M132" s="12"/>
+      <c r="N132" s="12"/>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A133" s="12" t="s">
         <v>117</v>
       </c>
@@ -21867,9 +22455,12 @@
       <c r="H133" s="12"/>
       <c r="I133" s="12"/>
       <c r="J133" s="12"/>
+      <c r="K133" s="12"/>
       <c r="L133" s="12"/>
-    </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M133" s="12"/>
+      <c r="N133" s="12"/>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A134" s="12" t="s">
         <v>118</v>
       </c>
@@ -21882,9 +22473,12 @@
       <c r="H134" s="12"/>
       <c r="I134" s="12"/>
       <c r="J134" s="12"/>
+      <c r="K134" s="12"/>
       <c r="L134" s="12"/>
-    </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M134" s="12"/>
+      <c r="N134" s="12"/>
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A135" s="12"/>
       <c r="B135" s="12"/>
       <c r="C135" s="12"/>
@@ -21895,9 +22489,12 @@
       <c r="H135" s="12"/>
       <c r="I135" s="12"/>
       <c r="J135" s="12"/>
+      <c r="K135" s="12"/>
       <c r="L135" s="12"/>
-    </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M135" s="12"/>
+      <c r="N135" s="12"/>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A136" s="13" t="s">
         <v>119</v>
       </c>
@@ -21910,9 +22507,12 @@
       <c r="H136" s="12"/>
       <c r="I136" s="12"/>
       <c r="J136" s="12"/>
+      <c r="K136" s="12"/>
       <c r="L136" s="12"/>
-    </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M136" s="12"/>
+      <c r="N136" s="12"/>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A137" s="12" t="s">
         <v>120</v>
       </c>
@@ -21925,9 +22525,12 @@
       <c r="H137" s="12"/>
       <c r="I137" s="12"/>
       <c r="J137" s="12"/>
+      <c r="K137" s="12"/>
       <c r="L137" s="12"/>
-    </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M137" s="12"/>
+      <c r="N137" s="12"/>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A138" s="12" t="s">
         <v>121</v>
       </c>
@@ -21940,9 +22543,12 @@
       <c r="H138" s="12"/>
       <c r="I138" s="12"/>
       <c r="J138" s="12"/>
+      <c r="K138" s="12"/>
       <c r="L138" s="12"/>
-    </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M138" s="12"/>
+      <c r="N138" s="12"/>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A139" s="12" t="s">
         <v>122</v>
       </c>
@@ -21955,9 +22561,12 @@
       <c r="H139" s="12"/>
       <c r="I139" s="12"/>
       <c r="J139" s="12"/>
+      <c r="K139" s="12"/>
       <c r="L139" s="12"/>
-    </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M139" s="12"/>
+      <c r="N139" s="12"/>
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A140" s="12" t="s">
         <v>123</v>
       </c>
@@ -21974,9 +22583,16 @@
       <c r="H140" s="12"/>
       <c r="I140" s="12"/>
       <c r="J140" s="12"/>
-      <c r="L140" s="12"/>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K140" s="12">
+        <v>111</v>
+      </c>
+      <c r="L140" s="12">
+        <v>200</v>
+      </c>
+      <c r="M140" s="12"/>
+      <c r="N140" s="12"/>
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A141" s="12" t="s">
         <v>266</v>
       </c>
@@ -21991,9 +22607,12 @@
       <c r="H141" s="12"/>
       <c r="I141" s="12"/>
       <c r="J141" s="12"/>
+      <c r="K141" s="12"/>
       <c r="L141" s="12"/>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M141" s="12"/>
+      <c r="N141" s="12"/>
+    </row>
+    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A142" s="12" t="s">
         <v>124</v>
       </c>
@@ -22006,9 +22625,12 @@
       <c r="H142" s="12"/>
       <c r="I142" s="12"/>
       <c r="J142" s="12"/>
+      <c r="K142" s="12"/>
       <c r="L142" s="12"/>
-    </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M142" s="12"/>
+      <c r="N142" s="12"/>
+    </row>
+    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A143" s="12" t="s">
         <v>125</v>
       </c>
@@ -22021,9 +22643,12 @@
       <c r="H143" s="12"/>
       <c r="I143" s="12"/>
       <c r="J143" s="12"/>
+      <c r="K143" s="12"/>
       <c r="L143" s="12"/>
-    </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M143" s="12"/>
+      <c r="N143" s="12"/>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A144" s="12" t="s">
         <v>207</v>
       </c>
@@ -22036,9 +22661,12 @@
       <c r="H144" s="12"/>
       <c r="I144" s="12"/>
       <c r="J144" s="12"/>
+      <c r="K144" s="12"/>
       <c r="L144" s="12"/>
-    </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M144" s="12"/>
+      <c r="N144" s="12"/>
+    </row>
+    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A145" s="12" t="s">
         <v>208</v>
       </c>
@@ -22051,9 +22679,12 @@
       <c r="H145" s="12"/>
       <c r="I145" s="12"/>
       <c r="J145" s="12"/>
+      <c r="K145" s="12"/>
       <c r="L145" s="12"/>
-    </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M145" s="12"/>
+      <c r="N145" s="12"/>
+    </row>
+    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A146" s="12" t="s">
         <v>259</v>
       </c>
@@ -22066,9 +22697,14 @@
       <c r="H146" s="12"/>
       <c r="I146" s="12"/>
       <c r="J146" s="12"/>
+      <c r="K146" s="12">
+        <v>222</v>
+      </c>
       <c r="L146" s="12"/>
-    </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M146" s="12"/>
+      <c r="N146" s="12"/>
+    </row>
+    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A147" s="12" t="s">
         <v>127</v>
       </c>
@@ -22085,9 +22721,14 @@
       <c r="J147" s="12">
         <v>111</v>
       </c>
+      <c r="K147" s="12">
+        <v>222</v>
+      </c>
       <c r="L147" s="12"/>
-    </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M147" s="12"/>
+      <c r="N147" s="12"/>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A148" s="12" t="s">
         <v>128</v>
       </c>
@@ -22100,9 +22741,12 @@
       <c r="H148" s="12"/>
       <c r="I148" s="12"/>
       <c r="J148" s="12"/>
+      <c r="K148" s="12"/>
       <c r="L148" s="12"/>
-    </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M148" s="12"/>
+      <c r="N148" s="12"/>
+    </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A149" s="12" t="s">
         <v>129</v>
       </c>
@@ -22115,9 +22759,14 @@
       <c r="H149" s="12"/>
       <c r="I149" s="12"/>
       <c r="J149" s="12"/>
+      <c r="K149" s="12">
+        <v>111</v>
+      </c>
       <c r="L149" s="12"/>
-    </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M149" s="12"/>
+      <c r="N149" s="12"/>
+    </row>
+    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A150" s="12" t="s">
         <v>130</v>
       </c>
@@ -22130,9 +22779,12 @@
       <c r="H150" s="12"/>
       <c r="I150" s="12"/>
       <c r="J150" s="12"/>
+      <c r="K150" s="12"/>
       <c r="L150" s="12"/>
-    </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M150" s="12"/>
+      <c r="N150" s="12"/>
+    </row>
+    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A151" s="12" t="s">
         <v>131</v>
       </c>
@@ -22145,9 +22797,12 @@
       <c r="H151" s="12"/>
       <c r="I151" s="12"/>
       <c r="J151" s="12"/>
+      <c r="K151" s="12"/>
       <c r="L151" s="12"/>
-    </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M151" s="12"/>
+      <c r="N151" s="12"/>
+    </row>
+    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A152" s="12" t="s">
         <v>132</v>
       </c>
@@ -22162,9 +22817,14 @@
       <c r="H152" s="12"/>
       <c r="I152" s="12"/>
       <c r="J152" s="12"/>
+      <c r="K152" s="12">
+        <v>333</v>
+      </c>
       <c r="L152" s="12"/>
-    </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M152" s="12"/>
+      <c r="N152" s="12"/>
+    </row>
+    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A153" s="12" t="s">
         <v>133</v>
       </c>
@@ -22189,9 +22849,18 @@
       <c r="J153" s="12">
         <v>1332</v>
       </c>
-      <c r="L153" s="12"/>
-    </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K153" s="12">
+        <v>4551</v>
+      </c>
+      <c r="L153" s="12">
+        <v>480</v>
+      </c>
+      <c r="M153" s="12">
+        <v>280</v>
+      </c>
+      <c r="N153" s="12"/>
+    </row>
+    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A154" s="12" t="s">
         <v>134</v>
       </c>
@@ -22216,9 +22885,18 @@
       <c r="J154" s="12">
         <v>1332</v>
       </c>
-      <c r="L154" s="12"/>
-    </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K154" s="12">
+        <v>666</v>
+      </c>
+      <c r="L154" s="12">
+        <v>200</v>
+      </c>
+      <c r="M154" s="12">
+        <v>80</v>
+      </c>
+      <c r="N154" s="12"/>
+    </row>
+    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A155" s="12" t="s">
         <v>135</v>
       </c>
@@ -22231,9 +22909,12 @@
       <c r="H155" s="12"/>
       <c r="I155" s="12"/>
       <c r="J155" s="12"/>
+      <c r="K155" s="12"/>
       <c r="L155" s="12"/>
-    </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M155" s="12"/>
+      <c r="N155" s="12"/>
+    </row>
+    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A156" s="12" t="s">
         <v>136</v>
       </c>
@@ -22258,9 +22939,18 @@
       <c r="J156" s="12">
         <v>1665</v>
       </c>
-      <c r="L156" s="12"/>
-    </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K156" s="12">
+        <v>666</v>
+      </c>
+      <c r="L156" s="12">
+        <v>3182</v>
+      </c>
+      <c r="M156" s="12">
+        <v>5250</v>
+      </c>
+      <c r="N156" s="12"/>
+    </row>
+    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A157" s="12" t="s">
         <v>137</v>
       </c>
@@ -22273,9 +22963,12 @@
       <c r="H157" s="12"/>
       <c r="I157" s="12"/>
       <c r="J157" s="12"/>
+      <c r="K157" s="12"/>
       <c r="L157" s="12"/>
-    </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M157" s="12"/>
+      <c r="N157" s="12"/>
+    </row>
+    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A158" s="12" t="s">
         <v>138</v>
       </c>
@@ -22288,9 +22981,12 @@
       <c r="H158" s="12"/>
       <c r="I158" s="12"/>
       <c r="J158" s="12"/>
+      <c r="K158" s="12"/>
       <c r="L158" s="12"/>
-    </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M158" s="12"/>
+      <c r="N158" s="12"/>
+    </row>
+    <row r="159" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A159" s="12" t="s">
         <v>139</v>
       </c>
@@ -22303,9 +22999,14 @@
       <c r="H159" s="12"/>
       <c r="I159" s="12"/>
       <c r="J159" s="12"/>
+      <c r="K159" s="12">
+        <v>5217</v>
+      </c>
       <c r="L159" s="12"/>
-    </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M159" s="12"/>
+      <c r="N159" s="12"/>
+    </row>
+    <row r="160" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A160" s="12" t="s">
         <v>140</v>
       </c>
@@ -22318,9 +23019,18 @@
       <c r="H160" s="12"/>
       <c r="I160" s="12"/>
       <c r="J160" s="12"/>
-      <c r="L160" s="12"/>
-    </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K160" s="12">
+        <v>222</v>
+      </c>
+      <c r="L160" s="12">
+        <v>400</v>
+      </c>
+      <c r="M160" s="12">
+        <v>40</v>
+      </c>
+      <c r="N160" s="12"/>
+    </row>
+    <row r="161" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A161" s="12" t="s">
         <v>141</v>
       </c>
@@ -22333,9 +23043,12 @@
       <c r="H161" s="12"/>
       <c r="I161" s="12"/>
       <c r="J161" s="12"/>
+      <c r="K161" s="12"/>
       <c r="L161" s="12"/>
-    </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M161" s="12"/>
+      <c r="N161" s="12"/>
+    </row>
+    <row r="162" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A162" s="12" t="s">
         <v>142</v>
       </c>
@@ -22348,9 +23061,12 @@
       <c r="H162" s="12"/>
       <c r="I162" s="12"/>
       <c r="J162" s="12"/>
+      <c r="K162" s="12"/>
       <c r="L162" s="12"/>
-    </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M162" s="12"/>
+      <c r="N162" s="12"/>
+    </row>
+    <row r="163" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A163" s="12" t="s">
         <v>143</v>
       </c>
@@ -22363,9 +23079,12 @@
       <c r="H163" s="12"/>
       <c r="I163" s="12"/>
       <c r="J163" s="12"/>
+      <c r="K163" s="12"/>
       <c r="L163" s="12"/>
-    </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M163" s="12"/>
+      <c r="N163" s="12"/>
+    </row>
+    <row r="164" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A164" s="12" t="s">
         <v>144</v>
       </c>
@@ -22378,9 +23097,12 @@
       <c r="H164" s="12"/>
       <c r="I164" s="12"/>
       <c r="J164" s="12"/>
+      <c r="K164" s="12"/>
       <c r="L164" s="12"/>
-    </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M164" s="12"/>
+      <c r="N164" s="12"/>
+    </row>
+    <row r="165" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A165" s="12" t="s">
         <v>145</v>
       </c>
@@ -22393,9 +23115,12 @@
       <c r="H165" s="12"/>
       <c r="I165" s="12"/>
       <c r="J165" s="12"/>
+      <c r="K165" s="12"/>
       <c r="L165" s="12"/>
-    </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M165" s="12"/>
+      <c r="N165" s="12"/>
+    </row>
+    <row r="166" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A166" s="12" t="s">
         <v>146</v>
       </c>
@@ -22410,9 +23135,16 @@
       <c r="H166" s="12"/>
       <c r="I166" s="12"/>
       <c r="J166" s="12"/>
-      <c r="L166" s="12"/>
-    </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K166" s="12">
+        <v>222</v>
+      </c>
+      <c r="L166" s="12">
+        <v>40</v>
+      </c>
+      <c r="M166" s="12"/>
+      <c r="N166" s="12"/>
+    </row>
+    <row r="167" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A167" s="12" t="s">
         <v>147</v>
       </c>
@@ -22431,9 +23163,14 @@
         <v>40</v>
       </c>
       <c r="J167" s="12"/>
+      <c r="K167" s="12">
+        <v>444</v>
+      </c>
       <c r="L167" s="12"/>
-    </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M167" s="12"/>
+      <c r="N167" s="12"/>
+    </row>
+    <row r="168" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A168" s="12" t="s">
         <v>148</v>
       </c>
@@ -22448,9 +23185,12 @@
       <c r="H168" s="12"/>
       <c r="I168" s="12"/>
       <c r="J168" s="12"/>
+      <c r="K168" s="12"/>
       <c r="L168" s="12"/>
-    </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M168" s="12"/>
+      <c r="N168" s="12"/>
+    </row>
+    <row r="169" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A169" s="12" t="s">
         <v>149</v>
       </c>
@@ -22469,9 +23209,14 @@
       <c r="J169" s="12">
         <v>111</v>
       </c>
+      <c r="K169" s="12">
+        <v>888</v>
+      </c>
       <c r="L169" s="12"/>
-    </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M169" s="12"/>
+      <c r="N169" s="12"/>
+    </row>
+    <row r="170" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A170" s="12" t="s">
         <v>150</v>
       </c>
@@ -22486,9 +23231,16 @@
         <v>80</v>
       </c>
       <c r="J170" s="12"/>
+      <c r="K170" s="12">
+        <v>444</v>
+      </c>
       <c r="L170" s="12"/>
-    </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M170" s="12">
+        <v>40</v>
+      </c>
+      <c r="N170" s="12"/>
+    </row>
+    <row r="171" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A171" s="12" t="s">
         <v>151</v>
       </c>
@@ -22501,9 +23253,16 @@
       <c r="H171" s="12"/>
       <c r="I171" s="12"/>
       <c r="J171" s="12"/>
-      <c r="L171" s="12"/>
-    </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K171" s="12">
+        <v>111</v>
+      </c>
+      <c r="L171" s="12">
+        <v>160</v>
+      </c>
+      <c r="M171" s="12"/>
+      <c r="N171" s="12"/>
+    </row>
+    <row r="172" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A172" s="12" t="s">
         <v>87</v>
       </c>
@@ -22528,9 +23287,18 @@
       <c r="J172" s="12">
         <v>333</v>
       </c>
-      <c r="L172" s="12"/>
-    </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K172" s="12">
+        <v>1998</v>
+      </c>
+      <c r="L172" s="12">
+        <v>560</v>
+      </c>
+      <c r="M172" s="12">
+        <v>80</v>
+      </c>
+      <c r="N172" s="12"/>
+    </row>
+    <row r="173" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A173" s="12" t="s">
         <v>152</v>
       </c>
@@ -22555,9 +23323,18 @@
       <c r="J173" s="12">
         <v>7000</v>
       </c>
-      <c r="L173" s="12"/>
-    </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K173" s="12">
+        <v>5000</v>
+      </c>
+      <c r="L173" s="12">
+        <v>3182</v>
+      </c>
+      <c r="M173" s="12">
+        <v>5250</v>
+      </c>
+      <c r="N173" s="12"/>
+    </row>
+    <row r="174" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A174" s="12"/>
       <c r="B174" s="12"/>
       <c r="C174" s="12"/>
@@ -22568,9 +23345,12 @@
       <c r="H174" s="12"/>
       <c r="I174" s="12"/>
       <c r="J174" s="12"/>
+      <c r="K174" s="12"/>
       <c r="L174" s="12"/>
-    </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M174" s="12"/>
+      <c r="N174" s="12"/>
+    </row>
+    <row r="175" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A175" s="13" t="s">
         <v>153</v>
       </c>
@@ -22583,9 +23363,12 @@
       <c r="H175" s="12"/>
       <c r="I175" s="12"/>
       <c r="J175" s="12"/>
+      <c r="K175" s="12"/>
       <c r="L175" s="12"/>
-    </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M175" s="12"/>
+      <c r="N175" s="12"/>
+    </row>
+    <row r="176" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A176" s="12" t="s">
         <v>154</v>
       </c>
@@ -22606,9 +23389,16 @@
       <c r="J176" s="12">
         <v>111</v>
       </c>
-      <c r="L176" s="12"/>
-    </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K176" s="12">
+        <v>1554</v>
+      </c>
+      <c r="L176" s="12">
+        <v>40</v>
+      </c>
+      <c r="M176" s="12"/>
+      <c r="N176" s="12"/>
+    </row>
+    <row r="177" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A177" s="12"/>
       <c r="B177" s="12"/>
       <c r="C177" s="12"/>
@@ -22619,9 +23409,12 @@
       <c r="H177" s="12"/>
       <c r="I177" s="12"/>
       <c r="J177" s="12"/>
+      <c r="K177" s="12"/>
       <c r="L177" s="12"/>
-    </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M177" s="12"/>
+      <c r="N177" s="12"/>
+    </row>
+    <row r="178" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A178" s="13" t="s">
         <v>155</v>
       </c>
@@ -22634,9 +23427,12 @@
       <c r="H178" s="12"/>
       <c r="I178" s="12"/>
       <c r="J178" s="12"/>
+      <c r="K178" s="12"/>
       <c r="L178" s="12"/>
-    </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M178" s="12"/>
+      <c r="N178" s="12"/>
+    </row>
+    <row r="179" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A179" s="12" t="s">
         <v>156</v>
       </c>
@@ -22649,9 +23445,12 @@
       <c r="H179" s="12"/>
       <c r="I179" s="12"/>
       <c r="J179" s="12"/>
+      <c r="K179" s="12"/>
       <c r="L179" s="12"/>
-    </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M179" s="12"/>
+      <c r="N179" s="12"/>
+    </row>
+    <row r="180" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A180" s="12" t="s">
         <v>87</v>
       </c>
@@ -22674,9 +23473,18 @@
       <c r="J180" s="12">
         <v>333</v>
       </c>
-      <c r="L180" s="12"/>
-    </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K180" s="12">
+        <v>333</v>
+      </c>
+      <c r="L180" s="12">
+        <v>200</v>
+      </c>
+      <c r="M180" s="12">
+        <v>120</v>
+      </c>
+      <c r="N180" s="12"/>
+    </row>
+    <row r="181" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A181" s="12"/>
       <c r="B181" s="12"/>
       <c r="C181" s="12"/>
@@ -22687,9 +23495,12 @@
       <c r="H181" s="12"/>
       <c r="I181" s="12"/>
       <c r="J181" s="12"/>
+      <c r="K181" s="12"/>
       <c r="L181" s="12"/>
-    </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M181" s="12"/>
+      <c r="N181" s="12"/>
+    </row>
+    <row r="182" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A182" s="13" t="s">
         <v>157</v>
       </c>
@@ -22702,9 +23513,12 @@
       <c r="H182" s="12"/>
       <c r="I182" s="12"/>
       <c r="J182" s="12"/>
+      <c r="K182" s="12"/>
       <c r="L182" s="12"/>
-    </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M182" s="12"/>
+      <c r="N182" s="12"/>
+    </row>
+    <row r="183" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A183" s="12" t="s">
         <v>158</v>
       </c>
@@ -22717,9 +23531,12 @@
       <c r="H183" s="12"/>
       <c r="I183" s="12"/>
       <c r="J183" s="12"/>
+      <c r="K183" s="12"/>
       <c r="L183" s="12"/>
-    </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M183" s="12"/>
+      <c r="N183" s="12"/>
+    </row>
+    <row r="184" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A184" s="12" t="s">
         <v>159</v>
       </c>
@@ -22734,9 +23551,12 @@
       <c r="H184" s="12"/>
       <c r="I184" s="12"/>
       <c r="J184" s="12"/>
+      <c r="K184" s="12"/>
       <c r="L184" s="12"/>
-    </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M184" s="12"/>
+      <c r="N184" s="12"/>
+    </row>
+    <row r="185" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A185" s="12" t="s">
         <v>160</v>
       </c>
@@ -22749,9 +23569,12 @@
       <c r="H185" s="12"/>
       <c r="I185" s="12"/>
       <c r="J185" s="12"/>
+      <c r="K185" s="12"/>
       <c r="L185" s="12"/>
-    </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M185" s="12"/>
+      <c r="N185" s="12"/>
+    </row>
+    <row r="186" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A186" s="12" t="s">
         <v>161</v>
       </c>
@@ -22764,9 +23587,12 @@
       <c r="H186" s="12"/>
       <c r="I186" s="12"/>
       <c r="J186" s="12"/>
+      <c r="K186" s="12"/>
       <c r="L186" s="12"/>
-    </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M186" s="12"/>
+      <c r="N186" s="12"/>
+    </row>
+    <row r="187" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A187" s="12" t="s">
         <v>162</v>
       </c>
@@ -22779,9 +23605,12 @@
       <c r="H187" s="12"/>
       <c r="I187" s="12"/>
       <c r="J187" s="12"/>
+      <c r="K187" s="12"/>
       <c r="L187" s="12"/>
-    </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M187" s="12"/>
+      <c r="N187" s="12"/>
+    </row>
+    <row r="188" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A188" s="12" t="s">
         <v>163</v>
       </c>
@@ -22796,9 +23625,12 @@
       <c r="H188" s="12"/>
       <c r="I188" s="12"/>
       <c r="J188" s="12"/>
+      <c r="K188" s="12"/>
       <c r="L188" s="12"/>
-    </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M188" s="12"/>
+      <c r="N188" s="12"/>
+    </row>
+    <row r="189" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A189" s="12" t="s">
         <v>87</v>
       </c>
@@ -22811,9 +23643,14 @@
       <c r="H189" s="12"/>
       <c r="I189" s="12"/>
       <c r="J189" s="12"/>
-      <c r="L189" s="12"/>
-    </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K189" s="12"/>
+      <c r="L189" s="12">
+        <v>3182</v>
+      </c>
+      <c r="M189" s="12"/>
+      <c r="N189" s="12"/>
+    </row>
+    <row r="190" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A190" s="12"/>
       <c r="B190" s="12"/>
       <c r="C190" s="12"/>
@@ -22824,9 +23661,12 @@
       <c r="H190" s="12"/>
       <c r="I190" s="12"/>
       <c r="J190" s="12"/>
+      <c r="K190" s="12"/>
       <c r="L190" s="12"/>
-    </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M190" s="12"/>
+      <c r="N190" s="12"/>
+    </row>
+    <row r="191" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A191" s="13" t="s">
         <v>164</v>
       </c>
@@ -22839,9 +23679,12 @@
       <c r="H191" s="12"/>
       <c r="I191" s="12"/>
       <c r="J191" s="12"/>
+      <c r="K191" s="12"/>
       <c r="L191" s="12"/>
-    </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M191" s="12"/>
+      <c r="N191" s="12"/>
+    </row>
+    <row r="192" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A192" s="12" t="s">
         <v>165</v>
       </c>
@@ -22854,9 +23697,12 @@
       <c r="H192" s="12"/>
       <c r="I192" s="12"/>
       <c r="J192" s="12"/>
+      <c r="K192" s="12"/>
       <c r="L192" s="12"/>
-    </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M192" s="12"/>
+      <c r="N192" s="12"/>
+    </row>
+    <row r="193" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A193" s="12" t="s">
         <v>166</v>
       </c>
@@ -22871,9 +23717,14 @@
       <c r="J193" s="12">
         <v>111</v>
       </c>
+      <c r="K193" s="12"/>
       <c r="L193" s="12"/>
-    </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M193" s="12">
+        <v>40</v>
+      </c>
+      <c r="N193" s="12"/>
+    </row>
+    <row r="194" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A194" s="12" t="s">
         <v>167</v>
       </c>
@@ -22886,9 +23737,12 @@
       <c r="H194" s="12"/>
       <c r="I194" s="12"/>
       <c r="J194" s="12"/>
+      <c r="K194" s="12"/>
       <c r="L194" s="12"/>
-    </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M194" s="12"/>
+      <c r="N194" s="12"/>
+    </row>
+    <row r="195" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A195" s="12" t="s">
         <v>168</v>
       </c>
@@ -22903,9 +23757,12 @@
       <c r="H195" s="12"/>
       <c r="I195" s="12"/>
       <c r="J195" s="12"/>
+      <c r="K195" s="12"/>
       <c r="L195" s="12"/>
-    </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M195" s="12"/>
+      <c r="N195" s="12"/>
+    </row>
+    <row r="196" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A196" s="12" t="s">
         <v>169</v>
       </c>
@@ -22922,9 +23779,12 @@
       <c r="J196" s="12">
         <v>111</v>
       </c>
+      <c r="K196" s="12"/>
       <c r="L196" s="12"/>
-    </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M196" s="12"/>
+      <c r="N196" s="12"/>
+    </row>
+    <row r="197" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A197" s="12" t="s">
         <v>170</v>
       </c>
@@ -22949,9 +23809,18 @@
       <c r="J197" s="12">
         <v>555</v>
       </c>
-      <c r="L197" s="12"/>
-    </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K197" s="12">
+        <v>999</v>
+      </c>
+      <c r="L197" s="12">
+        <v>120</v>
+      </c>
+      <c r="M197" s="12">
+        <v>160</v>
+      </c>
+      <c r="N197" s="12"/>
+    </row>
+    <row r="198" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A198" s="12" t="s">
         <v>171</v>
       </c>
@@ -22970,9 +23839,12 @@
       <c r="J198" s="12">
         <v>1110</v>
       </c>
+      <c r="K198" s="12"/>
       <c r="L198" s="12"/>
-    </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M198" s="12"/>
+      <c r="N198" s="12"/>
+    </row>
+    <row r="199" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A199" s="12"/>
       <c r="B199" s="12"/>
       <c r="C199" s="12"/>
@@ -22983,9 +23855,12 @@
       <c r="H199" s="12"/>
       <c r="I199" s="12"/>
       <c r="J199" s="12"/>
+      <c r="K199" s="12"/>
       <c r="L199" s="12"/>
-    </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M199" s="12"/>
+      <c r="N199" s="12"/>
+    </row>
+    <row r="200" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A200" s="12" t="s">
         <v>172</v>
       </c>
@@ -22998,9 +23873,12 @@
       <c r="H200" s="12"/>
       <c r="I200" s="12"/>
       <c r="J200" s="12"/>
+      <c r="K200" s="12"/>
       <c r="L200" s="12"/>
-    </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M200" s="12"/>
+      <c r="N200" s="12"/>
+    </row>
+    <row r="201" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A201" s="12" t="s">
         <v>173</v>
       </c>
@@ -23015,9 +23893,12 @@
       <c r="H201" s="12"/>
       <c r="I201" s="12"/>
       <c r="J201" s="12"/>
+      <c r="K201" s="12"/>
       <c r="L201" s="12"/>
-    </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M201" s="12"/>
+      <c r="N201" s="12"/>
+    </row>
+    <row r="202" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A202" s="12" t="s">
         <v>174</v>
       </c>
@@ -23030,9 +23911,14 @@
       <c r="H202" s="12"/>
       <c r="I202" s="12"/>
       <c r="J202" s="12"/>
+      <c r="K202" s="12"/>
       <c r="L202" s="12"/>
-    </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M202" s="12">
+        <v>40</v>
+      </c>
+      <c r="N202" s="12"/>
+    </row>
+    <row r="203" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A203" s="12"/>
       <c r="B203" s="12"/>
       <c r="C203" s="12"/>
@@ -23043,9 +23929,12 @@
       <c r="H203" s="12"/>
       <c r="I203" s="12"/>
       <c r="J203" s="12"/>
+      <c r="K203" s="12"/>
       <c r="L203" s="12"/>
-    </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M203" s="12"/>
+      <c r="N203" s="12"/>
+    </row>
+    <row r="204" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A204" s="12" t="s">
         <v>175</v>
       </c>
@@ -23058,9 +23947,12 @@
       <c r="H204" s="12"/>
       <c r="I204" s="12"/>
       <c r="J204" s="12"/>
+      <c r="K204" s="12"/>
       <c r="L204" s="12"/>
-    </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M204" s="12"/>
+      <c r="N204" s="12"/>
+    </row>
+    <row r="205" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A205" s="12" t="s">
         <v>176</v>
       </c>
@@ -23073,9 +23965,12 @@
       <c r="H205" s="12"/>
       <c r="I205" s="12"/>
       <c r="J205" s="12"/>
+      <c r="K205" s="12"/>
       <c r="L205" s="12"/>
-    </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M205" s="12"/>
+      <c r="N205" s="12"/>
+    </row>
+    <row r="206" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A206" s="12" t="s">
         <v>177</v>
       </c>
@@ -23092,9 +23987,14 @@
       <c r="J206" s="12">
         <v>3500</v>
       </c>
+      <c r="K206" s="12"/>
       <c r="L206" s="12"/>
-    </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M206" s="12">
+        <v>3500</v>
+      </c>
+      <c r="N206" s="12"/>
+    </row>
+    <row r="207" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A207" s="12" t="s">
         <v>177</v>
       </c>
@@ -23111,9 +24011,14 @@
       <c r="J207" s="12">
         <v>39888</v>
       </c>
+      <c r="K207" s="12">
+        <v>4329</v>
+      </c>
       <c r="L207" s="12"/>
-    </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M207" s="12"/>
+      <c r="N207" s="12"/>
+    </row>
+    <row r="208" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A208" s="12"/>
       <c r="B208" s="12"/>
       <c r="C208" s="12"/>
@@ -23124,9 +24029,12 @@
       <c r="H208" s="12"/>
       <c r="I208" s="12"/>
       <c r="J208" s="12"/>
+      <c r="K208" s="12"/>
       <c r="L208" s="12"/>
-    </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M208" s="12"/>
+      <c r="N208" s="12"/>
+    </row>
+    <row r="209" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A209" s="12" t="s">
         <v>179</v>
       </c>
@@ -23139,9 +24047,12 @@
       <c r="H209" s="12"/>
       <c r="I209" s="12"/>
       <c r="J209" s="12"/>
+      <c r="K209" s="12"/>
       <c r="L209" s="12"/>
-    </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M209" s="12"/>
+      <c r="N209" s="12"/>
+    </row>
+    <row r="210" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A210" s="12" t="s">
         <v>180</v>
       </c>
@@ -23154,9 +24065,12 @@
       <c r="H210" s="12"/>
       <c r="I210" s="12"/>
       <c r="J210" s="12"/>
+      <c r="K210" s="12"/>
       <c r="L210" s="12"/>
-    </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M210" s="12"/>
+      <c r="N210" s="12"/>
+    </row>
+    <row r="211" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A211" s="12"/>
       <c r="B211" s="12"/>
       <c r="C211" s="12"/>
@@ -23167,9 +24081,12 @@
       <c r="H211" s="12"/>
       <c r="I211" s="12"/>
       <c r="J211" s="12"/>
+      <c r="K211" s="12"/>
       <c r="L211" s="12"/>
-    </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M211" s="12"/>
+      <c r="N211" s="12"/>
+    </row>
+    <row r="212" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A212" s="12" t="s">
         <v>181</v>
       </c>
@@ -23194,9 +24111,18 @@
       <c r="J212" s="12">
         <v>343000</v>
       </c>
-      <c r="L212" s="12"/>
-    </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K212" s="12">
+        <v>270000</v>
+      </c>
+      <c r="L212" s="12">
+        <v>206830</v>
+      </c>
+      <c r="M212" s="12">
+        <v>75250</v>
+      </c>
+      <c r="N212" s="12"/>
+    </row>
+    <row r="213" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A213" s="12"/>
       <c r="B213" s="12"/>
       <c r="C213" s="12"/>
@@ -23207,9 +24133,12 @@
       <c r="H213" s="12"/>
       <c r="I213" s="12"/>
       <c r="J213" s="12"/>
+      <c r="K213" s="12"/>
       <c r="L213" s="12"/>
-    </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M213" s="12"/>
+      <c r="N213" s="12"/>
+    </row>
+    <row r="214" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A214" s="12" t="s">
         <v>182</v>
       </c>
@@ -23222,9 +24151,12 @@
       <c r="H214" s="12"/>
       <c r="I214" s="12"/>
       <c r="J214" s="12"/>
+      <c r="K214" s="12"/>
       <c r="L214" s="12"/>
-    </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M214" s="12"/>
+      <c r="N214" s="12"/>
+    </row>
+    <row r="215" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A215" s="12"/>
       <c r="B215" s="12"/>
       <c r="C215" s="12"/>
@@ -23235,9 +24167,12 @@
       <c r="H215" s="12"/>
       <c r="I215" s="12"/>
       <c r="J215" s="12"/>
+      <c r="K215" s="12"/>
       <c r="L215" s="12"/>
-    </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M215" s="12"/>
+      <c r="N215" s="12"/>
+    </row>
+    <row r="216" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A216" s="12" t="s">
         <v>183</v>
       </c>
@@ -23254,9 +24189,14 @@
       </c>
       <c r="I216" s="12"/>
       <c r="J216" s="12"/>
+      <c r="K216" s="12"/>
       <c r="L216" s="12"/>
-    </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M216" s="12">
+        <v>40</v>
+      </c>
+      <c r="N216" s="12"/>
+    </row>
+    <row r="217" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A217" s="12"/>
       <c r="B217" s="12"/>
       <c r="C217" s="12"/>
@@ -23267,9 +24207,9 @@
       <c r="H217" s="12"/>
       <c r="I217" s="12"/>
       <c r="J217" s="12"/>
-      <c r="L217" s="12"/>
-    </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N217" s="12"/>
+    </row>
+    <row r="218" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A218" s="12" t="s">
         <v>184</v>
       </c>
@@ -23286,9 +24226,9 @@
       <c r="J218" s="12" t="s">
         <v>269</v>
       </c>
-      <c r="L218" s="12"/>
-    </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="N218" s="12"/>
+    </row>
+    <row r="219" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A219" s="12"/>
       <c r="B219" s="12"/>
       <c r="C219" s="12"/>
@@ -23302,13 +24242,13 @@
         <v>270</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:14" x14ac:dyDescent="0.3">
       <c r="I220" s="12"/>
       <c r="J220" s="12" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:14" x14ac:dyDescent="0.3">
       <c r="I221" s="12"/>
       <c r="J221" s="12" t="s">
         <v>272</v>

</xml_diff>